<commit_message>
finishing the DQ paper with the evaluation section
</commit_message>
<xml_diff>
--- a/Papers/Towards An Objective Assessment Framework for Linked Data Quality/figures/LOD Result Analysis.xlsx
+++ b/Papers/Towards An Objective Assessment Framework for Linked Data Quality/figures/LOD Result Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19155" yWindow="0" windowWidth="19155" windowHeight="18240" tabRatio="500"/>
+    <workbookView xWindow="19155" yWindow="0" windowWidth="19155" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t xml:space="preserve">completeness      </t>
   </si>
@@ -85,9 +85,6 @@
     <t>QI.37</t>
   </si>
   <si>
-    <t>QI.38</t>
-  </si>
-  <si>
     <t>QI.39</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>QI.44</t>
   </si>
   <si>
-    <t>QI.46</t>
-  </si>
-  <si>
     <t>Quality Measure</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>Correctness</t>
   </si>
   <si>
-    <t>Comprehensibility</t>
-  </si>
-  <si>
     <t>Provenance</t>
   </si>
   <si>
@@ -140,6 +131,90 @@
   </si>
   <si>
     <t xml:space="preserve">Provenance        </t>
+  </si>
+  <si>
+    <t>QI.6</t>
+  </si>
+  <si>
+    <t>QI.5</t>
+  </si>
+  <si>
+    <t>QI.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports multiple serializations                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has different data access points                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uses datasets description vocabularies                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of descriptions about its size                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of descriptions about its structure (MIME Type, Format)          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of descriptions about its organization and categorization        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of dereferencable links for the dataset and its resources        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of an RDF dump that can be downloaded by users                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of queryable endpoints that respond to direct queries            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of valid dereferencable URLs (respond to HTTP request)           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of human and machine readable license information                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of dereferencable links to the full license information          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of timestamps that can keep track of its modifications           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes the correct MIME type for the content                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes the correct size for the content                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absence of Syntactic errors on the links level                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of at least one exemplary RDF file                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of general information (title, URL, description) for the dataset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of mailing list, message board or point of contact               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existence of metadata that describes its authoritative information         </t>
+  </si>
+  <si>
+    <t>QI.29</t>
+  </si>
+  <si>
+    <t>Use the HTTP URI Scheme</t>
+  </si>
+  <si>
+    <t>Comprehnsibility</t>
+  </si>
+  <si>
+    <t>QI.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usage of Versioning </t>
   </si>
 </sst>
 </file>
@@ -183,14 +258,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -198,6 +267,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,6 +298,228 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$24:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>completeness      </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>availability      </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>licensing         </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>freshness         </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correctness       </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>comprehensibility </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>provenance        </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.50219999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26219999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79490000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72060000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74070000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="174870912"/>
+        <c:axId val="174872832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="174870912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" b="0"/>
+                  <a:t>Quality Measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174872832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="174872832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6350">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" b="0"/>
+                  <a:t>Average Error %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="174870912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -247,9 +554,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$19</c:f>
+              <c:f>Sheet1!$B$1:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -260,118 +567,136 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$19</c:f>
+              <c:f>Sheet1!$C$1:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0.88649999999999995</c:v>
+                  <c:v>0.1135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80689999999999995</c:v>
+                  <c:v>0.19309999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.88800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41670000000000001</c:v>
+                  <c:v>0.86299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.8367</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.8417</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>0.96140000000000003</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.43190000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.83399999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>0.41020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.61580000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.99229999999999996</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.45900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.50700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.66579999999999995</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.98540000000000005</c:v>
+                  <c:v>0.2051</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>0.49099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.33450000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0.99609999999999999</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.43909999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
+                  <c:v>5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0.99609999999999999</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.78249999999999997</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.69879999999999998</c:v>
+                <c:pt idx="20">
+                  <c:v>0.2175</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.30120000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -386,11 +711,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133570560"/>
-        <c:axId val="133572096"/>
+        <c:axId val="174893312"/>
+        <c:axId val="174997888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133570560"/>
+        <c:axId val="174893312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,6 +745,7 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -433,7 +759,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133572096"/>
+        <c:crossAx val="174997888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -441,7 +767,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133572096"/>
+        <c:axId val="174997888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -483,229 +809,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133570560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Average Error</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$23:$A$29</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>completeness      </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>availability      </c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>licensing         </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>freshness         </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>correctness       </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>comprehensibility </c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>provenance        </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$23:$B$29</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.77759999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.745</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.60880000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.45900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.53959999999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.60780000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.49380000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="133612672"/>
-        <c:axId val="133614208"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="133612672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="fr-FR" b="0"/>
-                  <a:t>Quality Measure</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr rot="-5400000" vert="horz"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="133614208"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="133614208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="6350">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="fr-FR" b="0"/>
-                  <a:t>Average Error %</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133612672"/>
+        <c:crossAx val="174893312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -748,7 +852,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$35</c:f>
+              <c:f>Sheet2!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -760,9 +864,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -773,73 +877,91 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$35:$T$35</c:f>
+              <c:f>Sheet2!$B$2:$W$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0.88649999999999995</c:v>
+                  <c:v>0.1135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80689999999999995</c:v>
+                  <c:v>0.19309999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.88800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41670000000000001</c:v>
+                  <c:v>0.86299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8367</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4999999999999997E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -850,7 +972,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$36</c:f>
+              <c:f>Sheet2!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -862,9 +984,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -875,70 +997,79 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$36:$T$36</c:f>
+              <c:f>Sheet2!$B$3:$W$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="4" formatCode="0.00%">
+                <c:ptCount val="22"/>
+                <c:pt idx="7" formatCode="0.00%">
                   <c:v>0.8417</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00%">
+                <c:pt idx="8" formatCode="0.00%">
                   <c:v>0.96140000000000003</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.00%">
-                  <c:v>0.43190000000000001</c:v>
+                <c:pt idx="9" formatCode="0.00%">
+                  <c:v>0.41020000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -949,7 +1080,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$37</c:f>
+              <c:f>Sheet2!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -961,9 +1092,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -974,66 +1105,75 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$37:$T$37</c:f>
+              <c:f>Sheet2!$B$4:$W$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="7" formatCode="0.00%">
-                  <c:v>0.83399999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00%">
+                <c:ptCount val="22"/>
+                <c:pt idx="10" formatCode="0.00%">
+                  <c:v>0.61580000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00%">
                   <c:v>0.99229999999999996</c:v>
                 </c:pt>
               </c:numCache>
@@ -1045,7 +1185,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$38</c:f>
+              <c:f>Sheet2!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1057,9 +1197,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1070,64 +1210,73 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$38:$T$38</c:f>
+              <c:f>Sheet2!$B$5:$W$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="9" formatCode="0.00%">
-                  <c:v>0.45900000000000002</c:v>
+                <c:ptCount val="22"/>
+                <c:pt idx="12" formatCode="0.00%">
+                  <c:v>0.2051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1138,7 +1287,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$39</c:f>
+              <c:f>Sheet2!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1150,9 +1299,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1163,70 +1312,82 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$39:$T$39</c:f>
+              <c:f>Sheet2!$B$6:$W$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="10" formatCode="0.00%">
-                  <c:v>0.50700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00%">
-                  <c:v>0.66579999999999995</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00%">
-                  <c:v>0.98540000000000005</c:v>
+                <c:ptCount val="22"/>
+                <c:pt idx="13" formatCode="0.00%">
+                  <c:v>0.49099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00%">
+                  <c:v>0.33450000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00%">
+                  <c:v>1.2800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00%">
+                  <c:v>1.2800000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1237,7 +1398,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$40</c:f>
+              <c:f>Sheet2!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1249,9 +1410,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1262,72 +1423,78 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$40:$T$40</c:f>
+              <c:f>Sheet2!$B$7:$W$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="13" formatCode="0.00%">
+                <c:ptCount val="22"/>
+                <c:pt idx="17" formatCode="0.00%">
                   <c:v>0.99609999999999999</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0.00%">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.00%">
-                  <c:v>0.43909999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.00%">
+                <c:pt idx="18" formatCode="0.00%">
+                  <c:v>5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00%">
                   <c:v>0.99609999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -1339,7 +1506,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$41</c:f>
+              <c:f>Sheet2!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1351,9 +1518,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1364,67 +1531,76 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$41:$T$41</c:f>
+              <c:f>Sheet2!$B$8:$W$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="17" formatCode="0.00%">
-                  <c:v>0.78249999999999997</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="0.00%">
-                  <c:v>0.69879999999999998</c:v>
+                <c:ptCount val="22"/>
+                <c:pt idx="20" formatCode="0.00%">
+                  <c:v>0.2175</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00%">
+                  <c:v>0.30120000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,11 +1616,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="160862592"/>
-        <c:axId val="160865664"/>
+        <c:axId val="186337920"/>
+        <c:axId val="186356480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="160862592"/>
+        <c:axId val="186337920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,10 +1650,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160865664"/>
+        <c:crossAx val="186356480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1485,7 +1662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160865664"/>
+        <c:axId val="186356480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1495,7 +1672,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160862592"/>
+        <c:crossAx val="186337920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1543,7 +1720,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$35</c:f>
+              <c:f>Sheet2!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1555,9 +1732,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1568,73 +1745,91 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$35:$T$35</c:f>
+              <c:f>Sheet2!$B$2:$W$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0.88649999999999995</c:v>
+                  <c:v>0.1135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80689999999999995</c:v>
+                  <c:v>0.19309999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.88800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41670000000000001</c:v>
+                  <c:v>0.86299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8367</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4999999999999997E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1645,7 +1840,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$36</c:f>
+              <c:f>Sheet2!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1657,9 +1852,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1670,70 +1865,79 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$36:$T$36</c:f>
+              <c:f>Sheet2!$B$3:$W$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="4" formatCode="0.00%">
+                <c:ptCount val="22"/>
+                <c:pt idx="7" formatCode="0.00%">
                   <c:v>0.8417</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00%">
+                <c:pt idx="8" formatCode="0.00%">
                   <c:v>0.96140000000000003</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.00%">
-                  <c:v>0.43190000000000001</c:v>
+                <c:pt idx="9" formatCode="0.00%">
+                  <c:v>0.41020000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1744,7 +1948,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$37</c:f>
+              <c:f>Sheet2!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1756,9 +1960,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1769,66 +1973,75 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$37:$T$37</c:f>
+              <c:f>Sheet2!$B$4:$W$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="7" formatCode="0.00%">
-                  <c:v>0.83399999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00%">
+                <c:ptCount val="22"/>
+                <c:pt idx="10" formatCode="0.00%">
+                  <c:v>0.61580000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00%">
                   <c:v>0.99229999999999996</c:v>
                 </c:pt>
               </c:numCache>
@@ -1840,7 +2053,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$38</c:f>
+              <c:f>Sheet2!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1852,9 +2065,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1865,64 +2078,73 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$38:$T$38</c:f>
+              <c:f>Sheet2!$B$5:$W$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="9" formatCode="0.00%">
-                  <c:v>0.45900000000000002</c:v>
+                <c:ptCount val="22"/>
+                <c:pt idx="12" formatCode="0.00%">
+                  <c:v>0.2051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1933,7 +2155,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$39</c:f>
+              <c:f>Sheet2!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1945,9 +2167,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -1958,70 +2180,82 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$39:$T$39</c:f>
+              <c:f>Sheet2!$B$6:$W$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="10" formatCode="0.00%">
-                  <c:v>0.50700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00%">
-                  <c:v>0.66579999999999995</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00%">
-                  <c:v>0.98540000000000005</c:v>
+                <c:ptCount val="22"/>
+                <c:pt idx="13" formatCode="0.00%">
+                  <c:v>0.49099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00%">
+                  <c:v>0.33450000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00%">
+                  <c:v>1.2800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00%">
+                  <c:v>1.2800000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2032,7 +2266,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$40</c:f>
+              <c:f>Sheet2!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2044,9 +2278,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -2057,72 +2291,78 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$40:$T$40</c:f>
+              <c:f>Sheet2!$B$7:$W$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="13" formatCode="0.00%">
+                <c:ptCount val="22"/>
+                <c:pt idx="17" formatCode="0.00%">
                   <c:v>0.99609999999999999</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0.00%">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.00%">
-                  <c:v>0.43909999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.00%">
+                <c:pt idx="18" formatCode="0.00%">
+                  <c:v>5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00%">
                   <c:v>0.99609999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -2134,7 +2374,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$41</c:f>
+              <c:f>Sheet2!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2146,9 +2386,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$34:$T$34</c:f>
+              <c:f>Sheet2!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>QI.2</c:v>
                 </c:pt>
@@ -2159,67 +2399,76 @@
                   <c:v>QI.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>QI.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QI.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>QI.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>QI.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>QI.18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>QI.19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>QI.20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>QI.21</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>QI.22</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>QI.24</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>QI.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>QI.26</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>QI.28</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
+                  <c:v>QI.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>QI.37</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>QI.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>QI.39</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>QI.40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>QI.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>QI.46</c:v>
+                <c:pt idx="21">
+                  <c:v>QI.45</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$41:$T$41</c:f>
+              <c:f>Sheet2!$B$8:$W$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="17" formatCode="0.00%">
-                  <c:v>0.78249999999999997</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="0.00%">
-                  <c:v>0.69879999999999998</c:v>
+                <c:ptCount val="22"/>
+                <c:pt idx="20" formatCode="0.00%">
+                  <c:v>0.2175</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00%">
+                  <c:v>0.30120000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2234,11 +2483,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="122177408"/>
-        <c:axId val="122178944"/>
+        <c:axId val="188052608"/>
+        <c:axId val="188054528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="122177408"/>
+        <c:axId val="188052608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2263,10 +2512,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122178944"/>
+        <c:crossAx val="188054528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2274,7 +2524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122178944"/>
+        <c:axId val="188054528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2321,7 +2571,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="122177408"/>
+        <c:crossAx val="188052608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2353,20 +2603,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2383,21 +2633,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>708025</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2418,16 +2670,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2450,16 +2702,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1114424</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>128586</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>276224</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2803,290 +3055,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3">
-        <v>0.88649999999999995</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1">
+        <v>0.1135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.19309999999999999</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.8367</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.8417</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.96140000000000003</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.41020000000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.80689999999999995</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.88800000000000001</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.41670000000000001</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.8417</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.61580000000000001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.99229999999999996</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.96140000000000003</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.43190000000000001</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.83399999999999996</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.2051</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.99229999999999996</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.45900000000000002</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.33450000000000002</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="3">
-        <v>0.66579999999999995</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.98540000000000005</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.99609999999999999</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3">
+      <c r="B21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.2175</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.30120000000000002</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.43909999999999999</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0.99609999999999999</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0.78249999999999997</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="3">
-        <v>0.69879999999999998</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="3">
-        <f>AVERAGE(B1:B19)</f>
-        <v>0.71522105263157898</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0.77759999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" s="1">
+        <v>0.50219999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="3">
-        <v>0.745</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" s="1">
+        <v>0.26219999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="3">
-        <v>0.60880000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" s="1">
+        <v>0.19589999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="3">
-        <v>0.45900000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" s="1">
+        <v>0.79490000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="3">
-        <v>0.53959999999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" s="1">
+        <v>0.72060000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="3">
-        <v>0.60780000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" s="1">
+        <v>0.31619999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="3">
-        <v>0.49380000000000002</v>
+      <c r="B30" s="1">
+        <v>0.74070000000000003</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C19"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3097,173 +3434,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A34:T41"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="4" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="H1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M34" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N34" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O34" s="4" t="s">
+      <c r="R1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P34" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q34" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="R34" s="4" t="s">
+      <c r="V1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S34" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T34" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="W1" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.1135</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.19309999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.8367</v>
+      </c>
+      <c r="G2" s="1">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.8417</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.96140000000000003</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.41020000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.61580000000000001</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.99229999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0.2051</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0.33450000000000002</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1.2800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="3">
-        <v>0.88649999999999995</v>
-      </c>
-      <c r="C35" s="3">
-        <v>0.80689999999999995</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0.88800000000000001</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.41670000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="R7" s="1"/>
+      <c r="S7" s="1">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="T7" s="1">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0.99609999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="3">
-        <v>0.8417</v>
-      </c>
-      <c r="G36" s="3">
-        <v>0.96140000000000003</v>
-      </c>
-      <c r="H36" s="3">
-        <v>0.43190000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="I37" s="3">
-        <v>0.83399999999999996</v>
-      </c>
-      <c r="J37" s="3">
-        <v>0.99229999999999996</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>31</v>
-      </c>
-      <c r="K38" s="3">
-        <v>0.45900000000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="L39" s="3">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="M39" s="3">
-        <v>0.66579999999999995</v>
-      </c>
-      <c r="N39" s="3">
-        <v>0.98540000000000005</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="O40" s="3">
-        <v>0.99609999999999999</v>
-      </c>
-      <c r="P40" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="3">
-        <v>0.43909999999999999</v>
-      </c>
-      <c r="R40" s="3">
-        <v>0.99609999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="S41" s="3">
-        <v>0.78249999999999997</v>
-      </c>
-      <c r="T41" s="3">
-        <v>0.69879999999999998</v>
-      </c>
+      <c r="V8" s="1">
+        <v>0.2175</v>
+      </c>
+      <c r="W8" s="9">
+        <v>0.30120000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W34" s="2"/>
+    </row>
+    <row r="41" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>